<commit_message>
feature PrintPDF in QPP014
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp014a.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp014a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22035" windowHeight="6165" tabRatio="813"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22335" windowHeight="6150" tabRatio="813"/>
   </bookViews>
   <sheets>
     <sheet name="ケア対象者一覧" sheetId="25" r:id="rId1"/>
@@ -110,19 +110,19 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>&amp;=list.paymentMyn</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;=header.person(bean)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;=list.unit</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>&amp;=header.state(bean)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=list.paymentMyn</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=header.person(bean)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=list.unit</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -301,7 +301,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -349,6 +349,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -817,10 +820,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="D6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="16"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -833,50 +836,50 @@
       <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17" t="s">
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="17"/>
-      <c r="O7" s="20"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
@@ -891,28 +894,28 @@
       <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="19"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="22"/>
+      <c r="M9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="23"/>
       <c r="O9" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
qpp014: update export A
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp014a.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp014a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="6150" tabRatio="813"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22515" windowHeight="7560" tabRatio="813"/>
   </bookViews>
   <sheets>
     <sheet name="ケア対象者一覧" sheetId="25" r:id="rId1"/>
@@ -130,11 +130,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -142,14 +142,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -157,7 +157,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -197,33 +197,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -237,48 +215,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -307,7 +245,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -323,71 +261,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -716,48 +612,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="0.25" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="0.28515625" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="5" style="2" customWidth="1"/>
     <col min="8" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="10.75" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.75" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="2" customWidth="1"/>
     <col min="13" max="14" width="9" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.75" style="2" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="2" customWidth="1"/>
     <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="7"/>
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8"/>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -771,10 +667,10 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="9"/>
+      <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -788,10 +684,10 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="9"/>
+      <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -805,13 +701,13 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="9"/>
+      <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="3"/>
@@ -826,20 +722,20 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="10"/>
+      <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -849,104 +745,104 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="10"/>
+      <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:15" ht="9.75" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22" t="s">
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="22"/>
-      <c r="O7" s="23"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="26"/>
+    <row r="8" spans="1:15" ht="20.25" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:15" ht="20.25" customHeight="1">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="15" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="M9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="20"/>
-      <c r="O9" s="13" t="s">
+      <c r="N9" s="12"/>
+      <c r="O9" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:15" ht="20.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:I8"/>
+    <mergeCell ref="J7:L8"/>
     <mergeCell ref="M7:O8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G7:I8"/>
-    <mergeCell ref="J7:L8"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.47244094488188998" right="0.47244094488188998" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>